<commit_message>
Evidence of entry info
</commit_message>
<xml_diff>
--- a/xxfs/evidence.xlsx
+++ b/xxfs/evidence.xlsx
@@ -64,25 +64,25 @@
     <t>Community</t>
   </si>
   <si>
-    <t>ImageineLerning</t>
-  </si>
-  <si>
-    <t>iaa1c275fwntd765htsaqzffv262yxj99rr6pv8ddc</t>
-  </si>
-  <si>
-    <t>stars1c275fwntd765htsaqzffv262yxj99rr6qjspyc</t>
-  </si>
-  <si>
-    <t>juno1c275fwntd765htsaqzffv262yxj99rr6zuy8g4</t>
-  </si>
-  <si>
-    <t>uptick1c275fwntd765htsaqzffv262yxj99rr68gm8kc</t>
-  </si>
-  <si>
-    <t>omniflix1c275fwntd765htsaqzffv262yxj99rr6fsk9ch</t>
-  </si>
-  <si>
-    <t>gcx#2489</t>
+    <t>The Coding Squad</t>
+  </si>
+  <si>
+    <t>iaa1gtuu2ux5kvmprt8skyvhwmrth3xs84n9jy2jyl</t>
+  </si>
+  <si>
+    <t>stars1gtuu2ux5kvmprt8skyvhwmrth3xs84n9n6a7dl</t>
+  </si>
+  <si>
+    <t>juno1gtuu2ux5kvmprt8skyvhwmrth3xs84n935fcpj</t>
+  </si>
+  <si>
+    <t>uptick16m3p0ewytcqank0hnd82rp35tsqulmntjpgtfe</t>
+  </si>
+  <si>
+    <t>omniflix1gtuu2ux5kvmprt8skyvhwmrth3xs84n96cm63s</t>
+  </si>
+  <si>
+    <t>Axlvr#1089</t>
   </si>
   <si>
     <t>TxHash</t>
@@ -1140,7 +1140,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="7"/>

</xml_diff>

<commit_message>
fixed A2,A4 hash error
</commit_message>
<xml_diff>
--- a/xxfs/evidence.xlsx
+++ b/xxfs/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540" firstSheet="8" activeTab="20"/>
+    <workbookView windowWidth="28125" windowHeight="12540" firstSheet="8" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -2043,7 +2043,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
@@ -2122,8 +2122,8 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
@@ -2327,7 +2327,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -2379,7 +2379,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -2431,7 +2431,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -2460,7 +2460,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>21</v>
@@ -2483,7 +2483,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -2513,7 +2513,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>23</v>

</xml_diff>